<commit_message>
Excel to Parquet 2017-2023
</commit_message>
<xml_diff>
--- a/data/metadata/dicts/raw_SIMAT.xlsx
+++ b/data/metadata/dicts/raw_SIMAT.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanrengifo101/Documents/_trabajo/IDEA/school_dropout/data/metadata/dicts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariajoseguerrero/Documents/Secretaria de Educación/Deserción Escolar/school_dropout/data/metadata/dicts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C12F5AF-2BEC-D24A-8121-E4E374564D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7107072-D4C3-A348-B667-8BCA2934A940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="colname" sheetId="1" r:id="rId1"/>
     <sheet name="colclass" sheetId="2" r:id="rId2"/>
     <sheet name="Tablas" sheetId="4" r:id="rId3"/>
-    <sheet name="resumen" sheetId="3" r:id="rId4"/>
+    <sheet name="Clasificacion" sheetId="5" r:id="rId4"/>
+    <sheet name="resumen" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">colname!$A$1:$AL$1</definedName>
@@ -156,7 +157,7 @@
     <author>Maria Jose Guerrero</author>
   </authors>
   <commentList>
-    <comment ref="S4" authorId="0" shapeId="0" xr:uid="{6967ACD5-4B19-3645-BA61-FB51CE026CC8}">
+    <comment ref="Q4" authorId="0" shapeId="0" xr:uid="{6967ACD5-4B19-3645-BA61-FB51CE026CC8}">
       <text>
         <r>
           <rPr>
@@ -194,7 +195,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6337" uniqueCount="1017">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6406" uniqueCount="1017">
   <si>
     <t>uniname</t>
   </si>
@@ -3032,9 +3033,6 @@
   </si>
   <si>
     <t>no_doc_mad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tabla 1. Clasificación </t>
   </si>
   <si>
     <t>Tabla 2. Documentos e identificadores</t>
@@ -3257,6 +3255,9 @@
   </si>
   <si>
     <t>Grupo y curso al que pertenece</t>
+  </si>
+  <si>
+    <t>Tabla 1. Clasificacion</t>
   </si>
 </sst>
 </file>
@@ -3377,7 +3378,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -3423,17 +3424,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -3467,15 +3457,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -3493,17 +3474,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -3539,23 +3509,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3565,16 +3544,40 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3583,53 +3586,47 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3641,64 +3638,22 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4095,13 +4050,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL549"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView zoomScale="108" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="57.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="40.83203125" bestFit="1" customWidth="1"/>
     <col min="37" max="38" width="51.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4601,7 +4557,7 @@
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="24" t="s">
         <v>50</v>
       </c>
       <c r="C7" t="s">
@@ -4616,7 +4572,7 @@
       <c r="F7" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="24" t="s">
         <v>50</v>
       </c>
       <c r="H7" t="s">
@@ -14885,7 +14841,7 @@
       </c>
     </row>
     <row r="388" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A388" s="29" t="s">
+      <c r="A388" s="23" t="s">
         <v>532</v>
       </c>
       <c r="B388" t="s">
@@ -14905,7 +14861,7 @@
       </c>
     </row>
     <row r="389" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A389" s="29" t="s">
+      <c r="A389" s="23" t="s">
         <v>530</v>
       </c>
       <c r="B389" t="s">
@@ -14925,7 +14881,7 @@
       </c>
     </row>
     <row r="390" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A390" s="29" t="s">
+      <c r="A390" s="23" t="s">
         <v>528</v>
       </c>
       <c r="B390" t="s">
@@ -14945,7 +14901,7 @@
       </c>
     </row>
     <row r="391" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A391" s="29" t="s">
+      <c r="A391" s="23" t="s">
         <v>526</v>
       </c>
       <c r="B391" t="s">
@@ -15365,7 +15321,7 @@
       </c>
     </row>
     <row r="412" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A412" s="29" t="s">
+      <c r="A412" s="23" t="s">
         <v>490</v>
       </c>
       <c r="B412" t="s">
@@ -15385,7 +15341,7 @@
       </c>
     </row>
     <row r="413" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A413" s="29" t="s">
+      <c r="A413" s="23" t="s">
         <v>488</v>
       </c>
       <c r="B413" t="s">
@@ -15405,7 +15361,7 @@
       </c>
     </row>
     <row r="414" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A414" s="29" t="s">
+      <c r="A414" s="23" t="s">
         <v>486</v>
       </c>
       <c r="B414" t="s">
@@ -15465,7 +15421,7 @@
       </c>
     </row>
     <row r="417" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A417" s="29" t="s">
+      <c r="A417" s="23" t="s">
         <v>481</v>
       </c>
       <c r="B417" t="s">
@@ -16045,7 +16001,7 @@
       </c>
     </row>
     <row r="446" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A446" s="29" t="s">
+      <c r="A446" s="23" t="s">
         <v>440</v>
       </c>
       <c r="B446" t="s">
@@ -16065,7 +16021,7 @@
       </c>
     </row>
     <row r="447" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A447" s="29" t="s">
+      <c r="A447" s="23" t="s">
         <v>439</v>
       </c>
       <c r="B447" t="s">
@@ -16105,7 +16061,7 @@
       </c>
     </row>
     <row r="449" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A449" s="29" t="s">
+      <c r="A449" s="23" t="s">
         <v>436</v>
       </c>
       <c r="B449" t="s">
@@ -16125,7 +16081,7 @@
       </c>
     </row>
     <row r="450" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A450" s="29" t="s">
+      <c r="A450" s="23" t="s">
         <v>435</v>
       </c>
       <c r="B450" t="s">
@@ -16145,7 +16101,7 @@
       </c>
     </row>
     <row r="451" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A451" s="29" t="s">
+      <c r="A451" s="23" t="s">
         <v>434</v>
       </c>
       <c r="B451" t="s">
@@ -16165,7 +16121,7 @@
       </c>
     </row>
     <row r="452" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A452" s="29" t="s">
+      <c r="A452" s="23" t="s">
         <v>433</v>
       </c>
       <c r="B452" t="s">
@@ -16385,7 +16341,7 @@
       </c>
     </row>
     <row r="463" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A463" s="31" t="s">
+      <c r="A463" s="25" t="s">
         <v>415</v>
       </c>
       <c r="B463" t="s">
@@ -16465,7 +16421,7 @@
       </c>
     </row>
     <row r="467" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A467" s="29" t="s">
+      <c r="A467" s="23" t="s">
         <v>407</v>
       </c>
       <c r="B467" t="s">
@@ -16485,7 +16441,7 @@
       </c>
     </row>
     <row r="468" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A468" s="29" t="s">
+      <c r="A468" s="23" t="s">
         <v>405</v>
       </c>
       <c r="B468" t="s">
@@ -16505,7 +16461,7 @@
       </c>
     </row>
     <row r="469" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A469" s="29" t="s">
+      <c r="A469" s="23" t="s">
         <v>403</v>
       </c>
       <c r="B469" t="s">
@@ -16825,7 +16781,7 @@
       </c>
     </row>
     <row r="485" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A485" s="32" t="s">
+      <c r="A485" s="26" t="s">
         <v>381</v>
       </c>
       <c r="B485" t="s">
@@ -16885,7 +16841,7 @@
       </c>
     </row>
     <row r="488" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A488" s="32" t="s">
+      <c r="A488" s="26" t="s">
         <v>378</v>
       </c>
       <c r="B488" t="s">
@@ -17145,7 +17101,7 @@
       </c>
     </row>
     <row r="501" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A501" s="29" t="s">
+      <c r="A501" s="23" t="s">
         <v>363</v>
       </c>
       <c r="B501" t="s">
@@ -17165,7 +17121,7 @@
       </c>
     </row>
     <row r="502" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A502" s="29" t="s">
+      <c r="A502" s="23" t="s">
         <v>329</v>
       </c>
       <c r="B502" t="s">
@@ -17185,7 +17141,7 @@
       </c>
     </row>
     <row r="503" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A503" s="29" t="s">
+      <c r="A503" s="23" t="s">
         <v>328</v>
       </c>
       <c r="B503" t="s">
@@ -17205,7 +17161,7 @@
       </c>
     </row>
     <row r="504" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A504" s="29" t="s">
+      <c r="A504" s="23" t="s">
         <v>327</v>
       </c>
       <c r="B504" t="s">
@@ -17225,7 +17181,7 @@
       </c>
     </row>
     <row r="505" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A505" s="29" t="s">
+      <c r="A505" s="23" t="s">
         <v>326</v>
       </c>
       <c r="B505" t="s">
@@ -17245,7 +17201,7 @@
       </c>
     </row>
     <row r="506" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A506" s="29" t="s">
+      <c r="A506" s="23" t="s">
         <v>325</v>
       </c>
       <c r="B506" t="s">
@@ -17265,7 +17221,7 @@
       </c>
     </row>
     <row r="507" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A507" s="29" t="s">
+      <c r="A507" s="23" t="s">
         <v>324</v>
       </c>
       <c r="B507" t="s">
@@ -17285,7 +17241,7 @@
       </c>
     </row>
     <row r="508" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A508" s="29" t="s">
+      <c r="A508" s="23" t="s">
         <v>323</v>
       </c>
       <c r="B508" t="s">
@@ -17305,7 +17261,7 @@
       </c>
     </row>
     <row r="509" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A509" s="29" t="s">
+      <c r="A509" s="23" t="s">
         <v>322</v>
       </c>
       <c r="B509" t="s">
@@ -17325,7 +17281,7 @@
       </c>
     </row>
     <row r="510" spans="1:36" x14ac:dyDescent="0.2">
-      <c r="A510" s="29" t="s">
+      <c r="A510" s="23" t="s">
         <v>321</v>
       </c>
       <c r="B510" t="s">
@@ -17425,7 +17381,7 @@
       </c>
     </row>
     <row r="515" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A515" s="29" t="s">
+      <c r="A515" s="23" t="s">
         <v>356</v>
       </c>
       <c r="B515" t="s">
@@ -17445,7 +17401,7 @@
       </c>
     </row>
     <row r="516" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A516" s="29" t="s">
+      <c r="A516" s="23" t="s">
         <v>355</v>
       </c>
       <c r="B516" t="s">
@@ -17465,7 +17421,7 @@
       </c>
     </row>
     <row r="517" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A517" s="29" t="s">
+      <c r="A517" s="23" t="s">
         <v>354</v>
       </c>
       <c r="B517" t="s">
@@ -17485,7 +17441,7 @@
       </c>
     </row>
     <row r="518" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A518" s="29" t="s">
+      <c r="A518" s="23" t="s">
         <v>352</v>
       </c>
       <c r="B518" t="s">
@@ -17505,7 +17461,7 @@
       </c>
     </row>
     <row r="519" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A519" s="29" t="s">
+      <c r="A519" s="23" t="s">
         <v>351</v>
       </c>
       <c r="B519" t="s">
@@ -17525,7 +17481,7 @@
       </c>
     </row>
     <row r="520" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A520" s="29" t="s">
+      <c r="A520" s="23" t="s">
         <v>350</v>
       </c>
       <c r="B520" t="s">
@@ -17545,7 +17501,7 @@
       </c>
     </row>
     <row r="521" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A521" s="29" t="s">
+      <c r="A521" s="23" t="s">
         <v>349</v>
       </c>
       <c r="B521" t="s">
@@ -17565,7 +17521,7 @@
       </c>
     </row>
     <row r="522" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A522" s="29" t="s">
+      <c r="A522" s="23" t="s">
         <v>348</v>
       </c>
       <c r="B522" t="s">
@@ -17585,7 +17541,7 @@
       </c>
     </row>
     <row r="523" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A523" s="29" t="s">
+      <c r="A523" s="23" t="s">
         <v>347</v>
       </c>
       <c r="B523" t="s">
@@ -17605,7 +17561,7 @@
       </c>
     </row>
     <row r="524" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A524" s="29" t="s">
+      <c r="A524" s="23" t="s">
         <v>346</v>
       </c>
       <c r="B524" t="s">
@@ -17625,7 +17581,7 @@
       </c>
     </row>
     <row r="525" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A525" s="29" t="s">
+      <c r="A525" s="23" t="s">
         <v>345</v>
       </c>
       <c r="B525" t="s">
@@ -17645,7 +17601,7 @@
       </c>
     </row>
     <row r="526" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A526" s="29" t="s">
+      <c r="A526" s="23" t="s">
         <v>344</v>
       </c>
       <c r="B526" t="s">
@@ -17665,7 +17621,7 @@
       </c>
     </row>
     <row r="527" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A527" s="29" t="s">
+      <c r="A527" s="23" t="s">
         <v>334</v>
       </c>
       <c r="B527" t="s">
@@ -17685,7 +17641,7 @@
       </c>
     </row>
     <row r="528" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A528" s="29" t="s">
+      <c r="A528" s="23" t="s">
         <v>362</v>
       </c>
       <c r="B528" t="s">
@@ -17705,7 +17661,7 @@
       </c>
     </row>
     <row r="529" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A529" s="29" t="s">
+      <c r="A529" s="23" t="s">
         <v>343</v>
       </c>
       <c r="B529" t="s">
@@ -17725,7 +17681,7 @@
       </c>
     </row>
     <row r="530" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A530" s="29" t="s">
+      <c r="A530" s="23" t="s">
         <v>342</v>
       </c>
       <c r="B530" t="s">
@@ -17745,7 +17701,7 @@
       </c>
     </row>
     <row r="531" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A531" s="29" t="s">
+      <c r="A531" s="23" t="s">
         <v>341</v>
       </c>
       <c r="B531" t="s">
@@ -17765,7 +17721,7 @@
       </c>
     </row>
     <row r="532" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A532" s="29" t="s">
+      <c r="A532" s="23" t="s">
         <v>340</v>
       </c>
       <c r="B532" t="s">
@@ -17785,7 +17741,7 @@
       </c>
     </row>
     <row r="533" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A533" s="29" t="s">
+      <c r="A533" s="23" t="s">
         <v>339</v>
       </c>
       <c r="B533" t="s">
@@ -17805,7 +17761,7 @@
       </c>
     </row>
     <row r="534" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A534" s="29" t="s">
+      <c r="A534" s="23" t="s">
         <v>338</v>
       </c>
       <c r="B534" t="s">
@@ -17825,7 +17781,7 @@
       </c>
     </row>
     <row r="535" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A535" s="29" t="s">
+      <c r="A535" s="23" t="s">
         <v>336</v>
       </c>
       <c r="B535" t="s">
@@ -17845,7 +17801,7 @@
       </c>
     </row>
     <row r="536" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A536" s="29" t="s">
+      <c r="A536" s="23" t="s">
         <v>335</v>
       </c>
       <c r="B536" t="s">
@@ -17865,7 +17821,7 @@
       </c>
     </row>
     <row r="537" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A537" s="29" t="s">
+      <c r="A537" s="23" t="s">
         <v>333</v>
       </c>
       <c r="B537" t="s">
@@ -17885,7 +17841,7 @@
       </c>
     </row>
     <row r="538" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A538" s="29" t="s">
+      <c r="A538" s="23" t="s">
         <v>332</v>
       </c>
       <c r="B538" t="s">
@@ -17905,7 +17861,7 @@
       </c>
     </row>
     <row r="539" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A539" s="29" t="s">
+      <c r="A539" s="23" t="s">
         <v>361</v>
       </c>
       <c r="B539" t="s">
@@ -17925,7 +17881,7 @@
       </c>
     </row>
     <row r="540" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A540" s="29" t="s">
+      <c r="A540" s="23" t="s">
         <v>360</v>
       </c>
       <c r="B540" t="s">
@@ -17945,7 +17901,7 @@
       </c>
     </row>
     <row r="541" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A541" s="29" t="s">
+      <c r="A541" s="23" t="s">
         <v>359</v>
       </c>
       <c r="B541" t="s">
@@ -17965,7 +17921,7 @@
       </c>
     </row>
     <row r="542" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A542" s="29" t="s">
+      <c r="A542" s="23" t="s">
         <v>358</v>
       </c>
       <c r="B542" t="s">
@@ -17985,7 +17941,7 @@
       </c>
     </row>
     <row r="543" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A543" s="29" t="s">
+      <c r="A543" s="23" t="s">
         <v>357</v>
       </c>
       <c r="B543" t="s">
@@ -18005,7 +17961,7 @@
       </c>
     </row>
     <row r="544" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A544" s="29" t="s">
+      <c r="A544" s="23" t="s">
         <v>353</v>
       </c>
       <c r="B544" t="s">
@@ -18025,7 +17981,7 @@
       </c>
     </row>
     <row r="545" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A545" s="29" t="s">
+      <c r="A545" s="23" t="s">
         <v>337</v>
       </c>
       <c r="B545" t="s">
@@ -18045,7 +18001,7 @@
       </c>
     </row>
     <row r="546" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A546" s="29" t="s">
+      <c r="A546" s="23" t="s">
         <v>331</v>
       </c>
       <c r="B546" t="s">
@@ -18065,7 +18021,7 @@
       </c>
     </row>
     <row r="547" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A547" s="29" t="s">
+      <c r="A547" s="23" t="s">
         <v>330</v>
       </c>
       <c r="B547" t="s">
@@ -18085,7 +18041,7 @@
       </c>
     </row>
     <row r="548" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A548" s="29" t="s">
+      <c r="A548" s="23" t="s">
         <v>319</v>
       </c>
       <c r="B548" t="s">
@@ -18105,7 +18061,7 @@
       </c>
     </row>
     <row r="549" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A549" s="29" t="s">
+      <c r="A549" s="23" t="s">
         <v>320</v>
       </c>
       <c r="B549" t="s">
@@ -18143,6 +18099,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="34.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -25826,1832 +25785,1522 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A7E2DC-6F05-7D4E-8EC9-17ACA4EA4893}">
-  <dimension ref="B1:X83"/>
+  <dimension ref="B1:W83"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="167" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="6"/>
-    <col min="3" max="3" width="60.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="6"/>
-    <col min="6" max="6" width="36" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="6"/>
-    <col min="8" max="8" width="65.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="15" style="6" customWidth="1"/>
-    <col min="13" max="13" width="16.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.5" style="6" customWidth="1"/>
-    <col min="17" max="17" width="17.33203125" style="6" customWidth="1"/>
-    <col min="18" max="18" width="14.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.83203125" style="6"/>
-    <col min="21" max="21" width="15.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="10.83203125" style="6"/>
+    <col min="1" max="1" width="5.1640625" style="31" customWidth="1"/>
+    <col min="2" max="2" width="59" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.5" style="31" customWidth="1"/>
+    <col min="4" max="5" width="36" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="62.33203125" style="31" customWidth="1"/>
+    <col min="7" max="7" width="65.1640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="15" style="31" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" style="31" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.1640625" style="31" customWidth="1"/>
+    <col min="14" max="14" width="20.5" style="31" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5" style="31" customWidth="1"/>
+    <col min="16" max="16" width="17.33203125" style="31" customWidth="1"/>
+    <col min="17" max="17" width="14.1640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.33203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.1640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.33203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.1640625" style="31" customWidth="1"/>
+    <col min="22" max="22" width="14.6640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.1640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="10.83203125" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B1" s="33" t="s">
+    <row r="1" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B1" s="47" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C1" s="48"/>
+      <c r="D1" s="30"/>
+      <c r="F1" s="40" t="s">
         <v>946</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="35"/>
-      <c r="H1" s="36" t="s">
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="41"/>
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="30"/>
+    </row>
+    <row r="2" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B2" s="34" t="s">
         <v>947</v>
       </c>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="38"/>
-    </row>
-    <row r="2" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B2" s="33" t="s">
+      <c r="C2" s="27" t="s">
         <v>948</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="34" t="s">
+      <c r="F2" s="39" t="s">
+        <v>947</v>
+      </c>
+      <c r="G2" s="39" t="s">
         <v>949</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="H2" s="7" t="s">
-        <v>948</v>
-      </c>
-      <c r="I2" s="8" t="s">
+      <c r="H2" s="39" t="s">
         <v>950</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="39" t="s">
         <v>951</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="J2" s="39" t="s">
         <v>952</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="K2" s="39" t="s">
         <v>953</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="L2" s="39" t="s">
         <v>954</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="M2" s="39" t="s">
         <v>955</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="N2" s="39" t="s">
         <v>956</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="O2" s="39" t="s">
         <v>957</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="P2" s="39" t="s">
         <v>958</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="Q2" s="39" t="s">
         <v>959</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="R2" s="6" t="s">
         <v>960</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="S2" s="39" t="s">
         <v>961</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="T2" s="6" t="s">
         <v>962</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="U2" s="39" t="s">
         <v>963</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="V2" s="7" t="s">
         <v>964</v>
       </c>
-      <c r="X2" s="9" t="s">
+    </row>
+    <row r="3" spans="2:23" ht="32" x14ac:dyDescent="0.2">
+      <c r="B3" s="12" t="s">
         <v>965</v>
       </c>
-    </row>
-    <row r="3" spans="2:24" ht="32" x14ac:dyDescent="0.2">
-      <c r="B3" s="39" t="s">
+      <c r="C3" s="11" t="s">
         <v>966</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41" t="s">
+      <c r="F3" s="9" t="s">
+        <v>965</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="M3" s="10" t="s">
         <v>967</v>
       </c>
-      <c r="E3" s="40"/>
-      <c r="H3" s="10" t="s">
+      <c r="N3" s="10" t="s">
+        <v>968</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>853</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>732</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>734</v>
+      </c>
+      <c r="R3" s="28" t="s">
+        <v>736</v>
+      </c>
+      <c r="S3" s="9"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="8"/>
+    </row>
+    <row r="4" spans="2:23" ht="64" x14ac:dyDescent="0.2">
+      <c r="B4" s="12" t="s">
+        <v>969</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>966</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="N3" s="12" t="s">
+      <c r="F4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>383</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>385</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>382</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>863</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="M4" s="12"/>
+      <c r="N4" s="14" t="s">
+        <v>970</v>
+      </c>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12" t="s">
+        <v>367</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="R4" s="32"/>
+      <c r="S4" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="T4" s="32" t="s">
+        <v>374</v>
+      </c>
+      <c r="U4" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="V4" s="11" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>966</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="L5" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="O3" s="13" t="s">
-        <v>968</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>969</v>
-      </c>
-      <c r="Q3" s="12" t="s">
-        <v>853</v>
-      </c>
-      <c r="R3" s="12" t="s">
-        <v>732</v>
-      </c>
-      <c r="S3" s="12" t="s">
-        <v>734</v>
-      </c>
-      <c r="T3" s="12" t="s">
-        <v>736</v>
-      </c>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="11"/>
-    </row>
-    <row r="4" spans="2:24" ht="64" x14ac:dyDescent="0.2">
-      <c r="B4" s="42" t="s">
-        <v>970</v>
-      </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="44" t="s">
-        <v>967</v>
-      </c>
-      <c r="E4" s="43"/>
-      <c r="H4" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="16" t="s">
-        <v>383</v>
-      </c>
-      <c r="J4" s="16" t="s">
-        <v>385</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>382</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>384</v>
-      </c>
-      <c r="M4" s="17" t="s">
-        <v>863</v>
-      </c>
-      <c r="N4" s="16" t="s">
-        <v>378</v>
-      </c>
-      <c r="O4" s="16"/>
-      <c r="P4" s="18" t="s">
+      <c r="M5" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="32"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="11"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>966</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>880</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>744</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>541</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>861</v>
+      </c>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="32"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="11"/>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>966</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>730</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="M7" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="N7" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="32"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="11"/>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>966</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" s="13" t="s">
         <v>971</v>
       </c>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16" t="s">
-        <v>367</v>
-      </c>
-      <c r="S4" s="16" t="s">
-        <v>243</v>
-      </c>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16" t="s">
-        <v>375</v>
-      </c>
-      <c r="V4" s="16" t="s">
-        <v>374</v>
-      </c>
-      <c r="W4" s="16" t="s">
-        <v>380</v>
-      </c>
-      <c r="X4" s="15" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B5" s="42" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="44" t="s">
-        <v>967</v>
-      </c>
-      <c r="E5" s="43"/>
-      <c r="H5" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="17" t="s">
+      <c r="L8" s="13" t="s">
+        <v>742</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>539</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>857</v>
+      </c>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="32"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="11"/>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>966</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>972</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="N9" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="11"/>
+    </row>
+    <row r="10" spans="2:23" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>966</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>851</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>973</v>
+      </c>
+      <c r="M10" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="N10" s="18" t="s">
+        <v>974</v>
+      </c>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="R10" s="32"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="11"/>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B11" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>975</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="H11" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="I11" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="J11" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="M5" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="N5" s="17" t="s">
-        <v>294</v>
-      </c>
-      <c r="O5" s="17" t="s">
+      <c r="K11" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="M11" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="P5" s="17" t="s">
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="32"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="11"/>
+    </row>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>966</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="M12" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="N12" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="16"/>
-      <c r="W5" s="16"/>
-      <c r="X5" s="15"/>
-    </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B6" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="44" t="s">
-        <v>967</v>
-      </c>
-      <c r="E6" s="43"/>
-      <c r="H6" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="L6" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="M6" s="17" t="s">
-        <v>880</v>
-      </c>
-      <c r="N6" s="17" t="s">
-        <v>744</v>
-      </c>
-      <c r="O6" s="17" t="s">
-        <v>541</v>
-      </c>
-      <c r="P6" s="17" t="s">
-        <v>861</v>
-      </c>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="16"/>
-      <c r="X6" s="15"/>
-    </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B7" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="44" t="s">
-        <v>967</v>
-      </c>
-      <c r="E7" s="43"/>
-      <c r="H7" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="19" t="s">
-        <v>730</v>
-      </c>
-      <c r="J7" s="19" t="s">
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="32"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="11"/>
+    </row>
+    <row r="13" spans="2:23" ht="32" x14ac:dyDescent="0.2">
+      <c r="B13" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>966</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>976</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>977</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>978</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>979</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="L13" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="M13" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="N13" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="32"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="11"/>
+    </row>
+    <row r="14" spans="2:23" ht="32" x14ac:dyDescent="0.2">
+      <c r="B14" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>966</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>976</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>977</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>978</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>979</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="L14" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="32"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="11"/>
+    </row>
+    <row r="15" spans="2:23" ht="48" x14ac:dyDescent="0.2">
+      <c r="B15" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>975</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>972</v>
+      </c>
+      <c r="H15" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="K7" s="19" t="s">
+      <c r="I15" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="J15" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="M7" s="19" t="s">
+      <c r="K15" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="N7" s="19" t="s">
+      <c r="L15" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="O7" s="19" t="s">
+      <c r="M15" s="19" t="s">
+        <v>980</v>
+      </c>
+      <c r="N15" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="32"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="11"/>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B16" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>981</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="M16" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="P7" s="19" t="s">
+      <c r="N16" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="16"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="16"/>
-      <c r="X7" s="15"/>
-    </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B8" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="44" t="s">
-        <v>967</v>
-      </c>
-      <c r="E8" s="43"/>
-      <c r="H8" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="L8" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="M8" s="17" t="s">
-        <v>972</v>
-      </c>
-      <c r="N8" s="17" t="s">
-        <v>742</v>
-      </c>
-      <c r="O8" s="17" t="s">
-        <v>539</v>
-      </c>
-      <c r="P8" s="17" t="s">
-        <v>857</v>
-      </c>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="16"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="16"/>
-      <c r="X8" s="15"/>
-    </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B9" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="44" t="s">
-        <v>967</v>
-      </c>
-      <c r="E9" s="43"/>
-      <c r="H9" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>973</v>
-      </c>
-      <c r="J9" s="17" t="s">
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="32"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="11"/>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B17" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>981</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="K9" s="17" t="s">
+      <c r="I17" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="L9" s="17" t="s">
+      <c r="J17" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="M9" s="16"/>
-      <c r="N9" s="20" t="s">
+      <c r="K17" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="L17" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="O9" s="17" t="s">
+      <c r="M17" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="P9" s="17" t="s">
+      <c r="N17" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="16"/>
-      <c r="W9" s="16"/>
-      <c r="X9" s="15"/>
-    </row>
-    <row r="10" spans="2:24" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="42" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="44" t="s">
-        <v>967</v>
-      </c>
-      <c r="E10" s="43"/>
-      <c r="H10" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="J10" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="K10" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="L10" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="M10" s="21" t="s">
-        <v>851</v>
-      </c>
-      <c r="N10" s="22" t="s">
-        <v>974</v>
-      </c>
-      <c r="O10" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="P10" s="22" t="s">
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="32"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="32"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="11"/>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B18" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>981</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="M18" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="N18" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="32"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="32"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="11"/>
+    </row>
+    <row r="19" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B19" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>966</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="M19" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="N19" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="32"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="11"/>
+    </row>
+    <row r="20" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B20" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>975</v>
       </c>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="T10" s="16"/>
-      <c r="U10" s="16"/>
-      <c r="V10" s="16"/>
-      <c r="W10" s="16"/>
-      <c r="X10" s="15"/>
-    </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B11" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="44" t="s">
-        <v>976</v>
-      </c>
-      <c r="E11" s="43"/>
-      <c r="H11" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="16" t="s">
+      <c r="F20" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="H20" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="K11" s="17" t="s">
+      <c r="I20" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="L11" s="17" t="s">
+      <c r="J20" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="M11" s="17" t="s">
+      <c r="K20" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="N11" s="20" t="s">
+      <c r="L20" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="O11" s="17" t="s">
+      <c r="M20" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="16"/>
-      <c r="V11" s="16"/>
-      <c r="W11" s="16"/>
-      <c r="X11" s="15"/>
-    </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B12" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="44" t="s">
-        <v>967</v>
-      </c>
-      <c r="E12" s="43"/>
-      <c r="H12" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="17" t="s">
+      <c r="N20" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="32"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="11"/>
+    </row>
+    <row r="21" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B21" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>975</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="J12" s="17" t="s">
+      <c r="H21" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="K12" s="17" t="s">
+      <c r="I21" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="L12" s="17" t="s">
+      <c r="J21" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="M12" s="17" t="s">
+      <c r="K21" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="N12" s="17" t="s">
+      <c r="L21" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="O12" s="17" t="s">
+      <c r="M21" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="P12" s="17" t="s">
+      <c r="N21" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="16"/>
-      <c r="T12" s="16"/>
-      <c r="U12" s="16"/>
-      <c r="V12" s="16"/>
-      <c r="W12" s="16"/>
-      <c r="X12" s="15"/>
-    </row>
-    <row r="13" spans="2:24" ht="32" x14ac:dyDescent="0.2">
-      <c r="B13" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="44" t="s">
-        <v>967</v>
-      </c>
-      <c r="E13" s="43"/>
-      <c r="H13" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="23" t="s">
-        <v>977</v>
-      </c>
-      <c r="J13" s="23" t="s">
-        <v>978</v>
-      </c>
-      <c r="K13" s="23" t="s">
-        <v>979</v>
-      </c>
-      <c r="L13" s="23" t="s">
-        <v>980</v>
-      </c>
-      <c r="M13" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="N13" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="O13" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="P13" s="24" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q13" s="16"/>
-      <c r="R13" s="16"/>
-      <c r="S13" s="16"/>
-      <c r="T13" s="16"/>
-      <c r="U13" s="16"/>
-      <c r="V13" s="16"/>
-      <c r="W13" s="16"/>
-      <c r="X13" s="15"/>
-    </row>
-    <row r="14" spans="2:24" ht="32" x14ac:dyDescent="0.2">
-      <c r="B14" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="44" t="s">
-        <v>967</v>
-      </c>
-      <c r="E14" s="43"/>
-      <c r="H14" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>977</v>
-      </c>
-      <c r="J14" s="23" t="s">
-        <v>978</v>
-      </c>
-      <c r="K14" s="23" t="s">
-        <v>979</v>
-      </c>
-      <c r="L14" s="23" t="s">
-        <v>980</v>
-      </c>
-      <c r="M14" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="N14" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="O14" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="P14" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="16"/>
-      <c r="T14" s="16"/>
-      <c r="U14" s="16"/>
-      <c r="V14" s="16"/>
-      <c r="W14" s="16"/>
-      <c r="X14" s="15"/>
-    </row>
-    <row r="15" spans="2:24" ht="48" x14ac:dyDescent="0.2">
-      <c r="B15" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="43"/>
-      <c r="D15" s="44" t="s">
-        <v>976</v>
-      </c>
-      <c r="E15" s="43"/>
-      <c r="H15" s="14" t="s">
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="29"/>
+      <c r="U21" s="21"/>
+      <c r="V21" s="22"/>
+    </row>
+    <row r="22" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B22" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="16" t="s">
-        <v>973</v>
-      </c>
-      <c r="J15" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="K15" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="L15" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="M15" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="N15" s="24" t="s">
-        <v>128</v>
-      </c>
-      <c r="O15" s="23" t="s">
+      <c r="C22" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="23" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B23" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="24" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B24" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>981</v>
       </c>
-      <c r="P15" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q15" s="16"/>
-      <c r="R15" s="16"/>
-      <c r="S15" s="16"/>
-      <c r="T15" s="16"/>
-      <c r="U15" s="16"/>
-      <c r="V15" s="16"/>
-      <c r="W15" s="16"/>
-      <c r="X15" s="15"/>
-    </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B16" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="44" t="s">
+    </row>
+    <row r="25" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B25" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="26" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B26" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="27" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B27" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="28" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B28" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="29" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B29" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="30" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B30" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="31" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B31" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="32" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B32" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="43" t="s">
         <v>982</v>
       </c>
-      <c r="E16" s="43"/>
-      <c r="H16" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="I16" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="J16" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="K16" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="L16" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="M16" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="N16" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="O16" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="P16" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q16" s="16"/>
-      <c r="R16" s="16"/>
-      <c r="S16" s="16"/>
-      <c r="T16" s="16"/>
-      <c r="U16" s="16"/>
-      <c r="V16" s="16"/>
-      <c r="W16" s="16"/>
-      <c r="X16" s="15"/>
-    </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B17" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="44" t="s">
-        <v>982</v>
-      </c>
-      <c r="E17" s="43"/>
-      <c r="H17" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="J17" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="K17" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="L17" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="M17" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="N17" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="O17" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="P17" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
-      <c r="S17" s="16"/>
-      <c r="T17" s="16"/>
-      <c r="U17" s="16"/>
-      <c r="V17" s="16"/>
-      <c r="W17" s="16"/>
-      <c r="X17" s="15"/>
-    </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B18" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="43"/>
-      <c r="D18" s="44" t="s">
-        <v>982</v>
-      </c>
-      <c r="E18" s="43"/>
-      <c r="H18" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I18" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="J18" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="K18" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="L18" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="M18" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="N18" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="O18" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="P18" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q18" s="16"/>
-      <c r="R18" s="16"/>
-      <c r="S18" s="16"/>
-      <c r="T18" s="16"/>
-      <c r="U18" s="16"/>
-      <c r="V18" s="16"/>
-      <c r="W18" s="16"/>
-      <c r="X18" s="15"/>
-    </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B19" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="44" t="s">
-        <v>967</v>
-      </c>
-      <c r="E19" s="43"/>
-      <c r="H19" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="I19" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="J19" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="K19" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="L19" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="M19" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="N19" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="O19" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="P19" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="16"/>
-      <c r="S19" s="16"/>
-      <c r="T19" s="16"/>
-      <c r="U19" s="16"/>
-      <c r="V19" s="16"/>
-      <c r="W19" s="16"/>
-      <c r="X19" s="15"/>
-    </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B20" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="43"/>
-      <c r="D20" s="44" t="s">
-        <v>976</v>
-      </c>
-      <c r="E20" s="43"/>
-      <c r="H20" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="I20" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="K20" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="L20" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="M20" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="N20" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="O20" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="P20" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q20" s="16"/>
-      <c r="R20" s="16"/>
-      <c r="S20" s="16"/>
-      <c r="T20" s="16"/>
-      <c r="U20" s="16"/>
-      <c r="V20" s="16"/>
-      <c r="W20" s="16"/>
-      <c r="X20" s="15"/>
-    </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B21" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="44" t="s">
-        <v>976</v>
-      </c>
-      <c r="E21" s="43"/>
-      <c r="H21" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="I21" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="J21" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="K21" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="L21" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="M21" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="N21" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="O21" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="P21" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q21" s="26"/>
-      <c r="R21" s="26"/>
-      <c r="S21" s="26"/>
-      <c r="T21" s="26"/>
-      <c r="U21" s="26"/>
-      <c r="V21" s="26"/>
-      <c r="W21" s="26"/>
-      <c r="X21" s="27"/>
-    </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B22" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="43"/>
-      <c r="D22" s="44" t="s">
-        <v>967</v>
-      </c>
-      <c r="E22" s="43"/>
-    </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B23" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="44" t="s">
-        <v>976</v>
-      </c>
-      <c r="E23" s="43"/>
-    </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B24" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="43"/>
-      <c r="D24" s="44" t="s">
-        <v>982</v>
-      </c>
-      <c r="E24" s="43"/>
-    </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B25" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="43"/>
-      <c r="D25" s="44" t="s">
-        <v>982</v>
-      </c>
-      <c r="E25" s="43"/>
-    </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B26" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="43"/>
-      <c r="D26" s="44" t="s">
-        <v>967</v>
-      </c>
-      <c r="E26" s="43"/>
-    </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B27" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="43"/>
-      <c r="D27" s="44" t="s">
-        <v>967</v>
-      </c>
-      <c r="E27" s="43"/>
-    </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B28" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="43"/>
-      <c r="D28" s="44" t="s">
-        <v>967</v>
-      </c>
-      <c r="E28" s="43"/>
-    </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B29" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="43"/>
-      <c r="D29" s="44" t="s">
-        <v>982</v>
-      </c>
-      <c r="E29" s="43"/>
-    </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B30" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="43"/>
-      <c r="D30" s="44" t="s">
-        <v>982</v>
-      </c>
-      <c r="E30" s="43"/>
-    </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B31" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="43"/>
-      <c r="D31" s="44" t="s">
-        <v>967</v>
-      </c>
-      <c r="E31" s="43"/>
-    </row>
-    <row r="32" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B32" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="43"/>
-      <c r="D32" s="44" t="s">
-        <v>982</v>
-      </c>
-      <c r="E32" s="43"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B33" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" s="43"/>
-      <c r="D33" s="44" t="s">
-        <v>982</v>
-      </c>
-      <c r="E33" s="43"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B34" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="43"/>
-      <c r="D34" s="44" t="s">
-        <v>967</v>
-      </c>
-      <c r="E34" s="43"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B35" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="48"/>
-      <c r="D35" s="49" t="s">
-        <v>967</v>
-      </c>
-      <c r="E35" s="48"/>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B38" s="50" t="s">
+      <c r="C38" s="44"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="33"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="36" t="s">
         <v>983</v>
       </c>
-      <c r="C38" s="51"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="51"/>
-      <c r="F38" s="52"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B39" s="53" t="s">
+      <c r="C39" s="35" t="s">
         <v>984</v>
       </c>
-      <c r="C39" s="54"/>
-      <c r="D39" s="53" t="s">
+      <c r="D39" s="36" t="s">
         <v>985</v>
       </c>
-      <c r="E39" s="54"/>
-      <c r="F39" s="28" t="s">
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="C40" s="9" t="s">
         <v>986</v>
       </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B40" s="45" t="s">
-        <v>155</v>
-      </c>
-      <c r="C40" s="46"/>
-      <c r="D40" s="42" t="s">
+      <c r="D40" s="12" t="s">
         <v>987</v>
       </c>
-      <c r="E40" s="43"/>
-      <c r="F40" s="15" t="s">
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>986</v>
+      </c>
+      <c r="D41" s="12" t="s">
         <v>988</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="45" t="s">
-        <v>156</v>
-      </c>
-      <c r="C41" s="46"/>
-      <c r="D41" s="42" t="s">
-        <v>987</v>
-      </c>
-      <c r="E41" s="43"/>
-      <c r="F41" s="15" t="s">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>986</v>
+      </c>
+      <c r="D42" s="12" t="s">
         <v>989</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B42" s="45" t="s">
-        <v>157</v>
-      </c>
-      <c r="C42" s="46"/>
-      <c r="D42" s="42" t="s">
-        <v>987</v>
-      </c>
-      <c r="E42" s="43"/>
-      <c r="F42" s="15" t="s">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B43" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" s="12" t="s">
         <v>990</v>
       </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B43" s="45" t="s">
-        <v>158</v>
-      </c>
-      <c r="C43" s="46"/>
-      <c r="D43" s="42" t="s">
+      <c r="D43" s="12" t="s">
         <v>991</v>
       </c>
-      <c r="E43" s="43"/>
-      <c r="F43" s="15" t="s">
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>990</v>
+      </c>
+      <c r="D44" s="12" t="s">
         <v>992</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B44" s="45" t="s">
-        <v>162</v>
-      </c>
-      <c r="C44" s="46"/>
-      <c r="D44" s="42" t="s">
-        <v>991</v>
-      </c>
-      <c r="E44" s="43"/>
-      <c r="F44" s="15" t="s">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B45" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>986</v>
+      </c>
+      <c r="D45" s="12"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>986</v>
+      </c>
+      <c r="D46" s="12"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B47" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>990</v>
+      </c>
+      <c r="D47" s="12" t="s">
         <v>993</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B45" s="45" t="s">
-        <v>163</v>
-      </c>
-      <c r="C45" s="46"/>
-      <c r="D45" s="42" t="s">
-        <v>987</v>
-      </c>
-      <c r="E45" s="43"/>
-      <c r="F45" s="15"/>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B46" s="45" t="s">
-        <v>165</v>
-      </c>
-      <c r="C46" s="46"/>
-      <c r="D46" s="42" t="s">
-        <v>987</v>
-      </c>
-      <c r="E46" s="43"/>
-      <c r="F46" s="15"/>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B47" s="45" t="s">
-        <v>172</v>
-      </c>
-      <c r="C47" s="46"/>
-      <c r="D47" s="42" t="s">
-        <v>991</v>
-      </c>
-      <c r="E47" s="43"/>
-      <c r="F47" s="15" t="s">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B48" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="C48" s="12" t="s">
         <v>994</v>
       </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B48" s="45" t="s">
-        <v>173</v>
-      </c>
-      <c r="C48" s="46"/>
-      <c r="D48" s="42" t="s">
+      <c r="D48" s="12" t="s">
         <v>995</v>
       </c>
-      <c r="E48" s="43"/>
-      <c r="F48" s="15" t="s">
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B49" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>990</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B50" s="37" t="s">
+        <v>250</v>
+      </c>
+      <c r="C50" s="12" t="s">
         <v>996</v>
       </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B49" s="45" t="s">
-        <v>185</v>
-      </c>
-      <c r="C49" s="46"/>
-      <c r="D49" s="42" t="s">
-        <v>991</v>
-      </c>
-      <c r="E49" s="43"/>
-      <c r="F49" s="15" t="s">
+      <c r="D50" s="12" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B51" s="37" t="s">
+        <v>251</v>
+      </c>
+      <c r="C51" s="12" t="s">
         <v>996</v>
       </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B50" s="45" t="s">
-        <v>250</v>
-      </c>
-      <c r="C50" s="46"/>
-      <c r="D50" s="42" t="s">
+      <c r="D51" s="12" t="s">
         <v>997</v>
       </c>
-      <c r="E50" s="43"/>
-      <c r="F50" s="15" t="s">
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B52" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>990</v>
+      </c>
+      <c r="D52" s="12" t="s">
         <v>998</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B51" s="45" t="s">
-        <v>251</v>
-      </c>
-      <c r="C51" s="46"/>
-      <c r="D51" s="42" t="s">
-        <v>997</v>
-      </c>
-      <c r="E51" s="43"/>
-      <c r="F51" s="15" t="s">
-        <v>998</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B52" s="45" t="s">
-        <v>252</v>
-      </c>
-      <c r="C52" s="46"/>
-      <c r="D52" s="42" t="s">
-        <v>991</v>
-      </c>
-      <c r="E52" s="43"/>
-      <c r="F52" s="15" t="s">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B53" s="37" t="s">
+        <v>262</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>996</v>
+      </c>
+      <c r="D53" s="12" t="s">
         <v>999</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B53" s="45" t="s">
-        <v>262</v>
-      </c>
-      <c r="C53" s="46"/>
-      <c r="D53" s="42" t="s">
-        <v>997</v>
-      </c>
-      <c r="E53" s="43"/>
-      <c r="F53" s="15" t="s">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B54" s="37" t="s">
+        <v>269</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>990</v>
+      </c>
+      <c r="D54" s="12"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B55" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>990</v>
+      </c>
+      <c r="D55" s="12" t="s">
         <v>1000</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B54" s="45" t="s">
-        <v>269</v>
-      </c>
-      <c r="C54" s="46"/>
-      <c r="D54" s="42" t="s">
-        <v>991</v>
-      </c>
-      <c r="E54" s="43"/>
-      <c r="F54" s="15"/>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B55" s="45" t="s">
-        <v>271</v>
-      </c>
-      <c r="C55" s="46"/>
-      <c r="D55" s="42" t="s">
-        <v>991</v>
-      </c>
-      <c r="E55" s="43"/>
-      <c r="F55" s="15" t="s">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B56" s="37" t="s">
+        <v>277</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>990</v>
+      </c>
+      <c r="D56" s="12" t="s">
         <v>1001</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B56" s="45" t="s">
-        <v>277</v>
-      </c>
-      <c r="C56" s="46"/>
-      <c r="D56" s="42" t="s">
-        <v>991</v>
-      </c>
-      <c r="E56" s="43"/>
-      <c r="F56" s="15" t="s">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B57" s="37" t="s">
+        <v>279</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>990</v>
+      </c>
+      <c r="D57" s="12" t="s">
         <v>1002</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B57" s="45" t="s">
-        <v>279</v>
-      </c>
-      <c r="C57" s="46"/>
-      <c r="D57" s="42" t="s">
-        <v>991</v>
-      </c>
-      <c r="E57" s="43"/>
-      <c r="F57" s="15" t="s">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B58" s="37" t="s">
+        <v>286</v>
+      </c>
+      <c r="C58" s="12" t="s">
+        <v>990</v>
+      </c>
+      <c r="D58" s="12" t="s">
         <v>1003</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B58" s="45" t="s">
-        <v>286</v>
-      </c>
-      <c r="C58" s="46"/>
-      <c r="D58" s="42" t="s">
-        <v>991</v>
-      </c>
-      <c r="E58" s="43"/>
-      <c r="F58" s="15" t="s">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B59" s="37" t="s">
+        <v>288</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>986</v>
+      </c>
+      <c r="D59" s="12"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B60" s="37" t="s">
+        <v>303</v>
+      </c>
+      <c r="C60" s="12" t="s">
+        <v>996</v>
+      </c>
+      <c r="D60" s="12" t="s">
         <v>1004</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B59" s="45" t="s">
-        <v>288</v>
-      </c>
-      <c r="C59" s="46"/>
-      <c r="D59" s="42" t="s">
-        <v>987</v>
-      </c>
-      <c r="E59" s="43"/>
-      <c r="F59" s="15"/>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B60" s="45" t="s">
-        <v>303</v>
-      </c>
-      <c r="C60" s="46"/>
-      <c r="D60" s="42" t="s">
-        <v>997</v>
-      </c>
-      <c r="E60" s="43"/>
-      <c r="F60" s="15" t="s">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B61" s="37" t="s">
+        <v>304</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>996</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B62" s="37" t="s">
+        <v>307</v>
+      </c>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B63" s="37" t="s">
+        <v>373</v>
+      </c>
+      <c r="C63" s="12" t="s">
+        <v>986</v>
+      </c>
+      <c r="D63" s="12" t="s">
         <v>1005</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B61" s="45" t="s">
-        <v>304</v>
-      </c>
-      <c r="C61" s="46"/>
-      <c r="D61" s="42" t="s">
-        <v>997</v>
-      </c>
-      <c r="E61" s="43"/>
-      <c r="F61" s="15" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B62" s="45" t="s">
-        <v>307</v>
-      </c>
-      <c r="C62" s="46"/>
-      <c r="D62" s="42"/>
-      <c r="E62" s="43"/>
-      <c r="F62" s="15"/>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B63" s="45" t="s">
-        <v>373</v>
-      </c>
-      <c r="C63" s="46"/>
-      <c r="D63" s="42" t="s">
-        <v>987</v>
-      </c>
-      <c r="E63" s="43"/>
-      <c r="F63" s="15" t="s">
+    <row r="64" spans="2:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="37" t="s">
+        <v>400</v>
+      </c>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B65" s="37" t="s">
+        <v>427</v>
+      </c>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B66" s="37" t="s">
+        <v>445</v>
+      </c>
+      <c r="C66" s="12" t="s">
+        <v>990</v>
+      </c>
+      <c r="D66" s="12" t="s">
         <v>1006</v>
       </c>
     </row>
-    <row r="64" spans="2:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="45" t="s">
-        <v>400</v>
-      </c>
-      <c r="C64" s="46"/>
-      <c r="D64" s="42"/>
-      <c r="E64" s="43"/>
-      <c r="F64" s="15"/>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B65" s="45" t="s">
-        <v>427</v>
-      </c>
-      <c r="C65" s="46"/>
-      <c r="D65" s="42"/>
-      <c r="E65" s="43"/>
-      <c r="F65" s="15"/>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B66" s="45" t="s">
-        <v>445</v>
-      </c>
-      <c r="C66" s="46"/>
-      <c r="D66" s="42" t="s">
-        <v>991</v>
-      </c>
-      <c r="E66" s="43"/>
-      <c r="F66" s="15" t="s">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B67" s="37" t="s">
+        <v>515</v>
+      </c>
+      <c r="C67" s="12" t="s">
+        <v>986</v>
+      </c>
+      <c r="D67" s="12" t="s">
         <v>1007</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B67" s="45" t="s">
-        <v>515</v>
-      </c>
-      <c r="C67" s="46"/>
-      <c r="D67" s="42" t="s">
-        <v>987</v>
-      </c>
-      <c r="E67" s="43"/>
-      <c r="F67" s="15" t="s">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B68" s="37" t="s">
+        <v>516</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>986</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B69" s="37" t="s">
+        <v>517</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>986</v>
+      </c>
+      <c r="D69" s="12" t="s">
         <v>1008</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B68" s="45" t="s">
-        <v>516</v>
-      </c>
-      <c r="C68" s="46"/>
-      <c r="D68" s="42" t="s">
-        <v>987</v>
-      </c>
-      <c r="E68" s="43"/>
-      <c r="F68" s="15" t="s">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B69" s="45" t="s">
-        <v>517</v>
-      </c>
-      <c r="C69" s="46"/>
-      <c r="D69" s="42" t="s">
-        <v>987</v>
-      </c>
-      <c r="E69" s="43"/>
-      <c r="F69" s="15" t="s">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B70" s="37" t="s">
+        <v>520</v>
+      </c>
+      <c r="C70" s="12" t="s">
+        <v>986</v>
+      </c>
+      <c r="D70" s="12" t="s">
         <v>1009</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B70" s="45" t="s">
-        <v>520</v>
-      </c>
-      <c r="C70" s="46"/>
-      <c r="D70" s="42" t="s">
-        <v>987</v>
-      </c>
-      <c r="E70" s="43"/>
-      <c r="F70" s="15" t="s">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B71" s="37" t="s">
+        <v>522</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>986</v>
+      </c>
+      <c r="D71" s="12" t="s">
         <v>1010</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B71" s="45" t="s">
-        <v>522</v>
-      </c>
-      <c r="C71" s="46"/>
-      <c r="D71" s="42" t="s">
-        <v>987</v>
-      </c>
-      <c r="E71" s="43"/>
-      <c r="F71" s="15" t="s">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B72" s="37" t="s">
+        <v>563</v>
+      </c>
+      <c r="C72" s="12" t="s">
+        <v>990</v>
+      </c>
+      <c r="D72" s="12" t="s">
         <v>1011</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B72" s="45" t="s">
-        <v>563</v>
-      </c>
-      <c r="C72" s="46"/>
-      <c r="D72" s="42" t="s">
-        <v>991</v>
-      </c>
-      <c r="E72" s="43"/>
-      <c r="F72" s="15" t="s">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B73" s="37" t="s">
+        <v>564</v>
+      </c>
+      <c r="C73" s="12" t="s">
+        <v>990</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B74" s="37" t="s">
+        <v>565</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>990</v>
+      </c>
+      <c r="D74" s="12" t="s">
         <v>1012</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B73" s="45" t="s">
-        <v>564</v>
-      </c>
-      <c r="C73" s="46"/>
-      <c r="D73" s="42" t="s">
-        <v>991</v>
-      </c>
-      <c r="E73" s="43"/>
-      <c r="F73" s="15" t="s">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B74" s="45" t="s">
-        <v>565</v>
-      </c>
-      <c r="C74" s="46"/>
-      <c r="D74" s="42" t="s">
-        <v>991</v>
-      </c>
-      <c r="E74" s="43"/>
-      <c r="F74" s="15" t="s">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B75" s="37" t="s">
+        <v>595</v>
+      </c>
+      <c r="C75" s="12" t="s">
         <v>1013</v>
       </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B75" s="45" t="s">
-        <v>595</v>
-      </c>
-      <c r="C75" s="46"/>
-      <c r="D75" s="42" t="s">
+      <c r="D75" s="12" t="s">
         <v>1014</v>
       </c>
-      <c r="E75" s="43"/>
-      <c r="F75" s="15" t="s">
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B76" s="37" t="s">
+        <v>598</v>
+      </c>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B77" s="37" t="s">
+        <v>640</v>
+      </c>
+      <c r="C77" s="12" t="s">
+        <v>986</v>
+      </c>
+      <c r="D77" s="12"/>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B78" s="38" t="s">
+        <v>647</v>
+      </c>
+      <c r="C78" s="21" t="s">
+        <v>986</v>
+      </c>
+      <c r="D78" s="21" t="s">
         <v>1015</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B76" s="45" t="s">
-        <v>598</v>
-      </c>
-      <c r="C76" s="46"/>
-      <c r="D76" s="42"/>
-      <c r="E76" s="43"/>
-      <c r="F76" s="15"/>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B77" s="45" t="s">
-        <v>640</v>
-      </c>
-      <c r="C77" s="46"/>
-      <c r="D77" s="42" t="s">
-        <v>987</v>
-      </c>
-      <c r="E77" s="43"/>
-      <c r="F77" s="15"/>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B78" s="55" t="s">
-        <v>647</v>
-      </c>
-      <c r="C78" s="56"/>
-      <c r="D78" s="47" t="s">
-        <v>987</v>
-      </c>
-      <c r="E78" s="48"/>
-      <c r="F78" s="27" t="s">
-        <v>1016</v>
-      </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B79" s="57"/>
-      <c r="C79" s="57"/>
-      <c r="D79" s="58"/>
-      <c r="E79" s="58"/>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B80" s="57"/>
-      <c r="C80" s="57"/>
-      <c r="D80" s="58"/>
-      <c r="E80" s="58"/>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B81" s="57"/>
-      <c r="C81" s="57"/>
-      <c r="D81" s="58"/>
-      <c r="E81" s="58"/>
-    </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B82" s="57"/>
-      <c r="C82" s="57"/>
-      <c r="D82" s="58"/>
-      <c r="E82" s="58"/>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B83" s="57"/>
-      <c r="C83" s="57"/>
-      <c r="D83" s="58"/>
-      <c r="E83" s="58"/>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B79" s="46"/>
+      <c r="C79" s="46"/>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B80" s="46"/>
+      <c r="C80" s="46"/>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B81" s="46"/>
+      <c r="C81" s="46"/>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B82" s="46"/>
+      <c r="C82" s="46"/>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B83" s="46"/>
+      <c r="C83" s="46"/>
     </row>
   </sheetData>
-  <mergeCells count="161">
+  <mergeCells count="8">
+    <mergeCell ref="F1:V1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B38:D38"/>
     <mergeCell ref="B82:C82"/>
-    <mergeCell ref="D82:E82"/>
     <mergeCell ref="B83:C83"/>
-    <mergeCell ref="D83:E83"/>
     <mergeCell ref="B79:C79"/>
-    <mergeCell ref="D79:E79"/>
     <mergeCell ref="B80:C80"/>
-    <mergeCell ref="D80:E80"/>
     <mergeCell ref="B81:C81"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="H1:X1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -27659,6 +27308,297 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70D70565-0FB9-2544-B2AF-582EA7457899}">
+  <dimension ref="A1:B34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="34" t="s">
+        <v>947</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>969</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>966</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1435D5A1-0AC9-6D49-8B79-0AC50D35E22C}">
   <dimension ref="B2:N12"/>
   <sheetViews>

</xml_diff>